<commit_message>
Ran API tests for the services routes. Updated spreadsheet to reflect testing status.
</commit_message>
<xml_diff>
--- a/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
+++ b/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6988A331-6A60-41FE-BB44-2EC11A5567A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB95B003-7625-4826-BBFF-5AF0BD9C1A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="Lists" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$O$49</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="307">
   <si>
     <t>TC_ID</t>
   </si>
@@ -877,21 +877,12 @@
     <t>Robert Norwood</t>
   </si>
   <si>
-    <t>2026-01-16</t>
-  </si>
-  <si>
-    <t>Manual API test via Postman</t>
-  </si>
-  <si>
     <t>Create service (valid payload)</t>
   </si>
   <si>
     <t>1) Send POST /api/services with valid JSON body</t>
   </si>
   <si>
-    <t>{"name":"En Vogue Finish","description":"Luxury bath + blow dry.","image":"https://example.com/service.jpg","price":95,"durationMins":90}</t>
-  </si>
-  <si>
     <t>201 Created; success=true; data contains created service with _id; service persisted in DB</t>
   </si>
   <si>
@@ -907,9 +898,6 @@
     <t>400 Bad Request; success=false; message indicates invalid service data; no DB insert</t>
   </si>
   <si>
-    <t>Validates Joi schema on create</t>
-  </si>
-  <si>
     <t>Get service by id returns service</t>
   </si>
   <si>
@@ -937,9 +925,6 @@
     <t>400 Bad Request; success=false; message indicates invalid service id</t>
   </si>
   <si>
-    <t>Prevents DB call when id is invalid</t>
-  </si>
-  <si>
     <t>Update service (valid update)</t>
   </si>
   <si>
@@ -955,9 +940,6 @@
     <t>200 OK; success=true; returned data reflects updated fields; DB updated</t>
   </si>
   <si>
-    <t>Uses Joi validation + Mongoose runValidators</t>
-  </si>
-  <si>
     <t>Delete service removes service</t>
   </si>
   <si>
@@ -982,9 +964,6 @@
     <t>404 Not Found; success=false; message indicates service not found</t>
   </si>
   <si>
-    <t>Confirms deletion effect</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -1013,6 +992,31 @@
   </si>
   <si>
     <t>TC-048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "name": "Testing Service Creation",
+  "description": "new grooming service here!",
+  "image": "https://example.com/service.jpg",
+  "price": 55,
+  "durationMins": 30
+}
+</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms deletion effect.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Uses Joi validation + Mongoose runValidators.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Prevents DB call when id is invalid.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Validates Joi schema on create.</t>
   </si>
 </sst>
 </file>
@@ -1020,9 +1024,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1038,8 +1042,17 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1065,16 +1078,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFD9D9D9"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FFD9D9D9"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FFD9D9D9"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFD9D9D9"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1082,27 +1095,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFE0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1401,2015 +1441,2026 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="5" customWidth="1"/>
-    <col min="7" max="7" width="53.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="42" style="5" customWidth="1"/>
-    <col min="9" max="9" width="24" style="5" customWidth="1"/>
-    <col min="10" max="10" width="32" style="5" customWidth="1"/>
-    <col min="11" max="11" width="22" style="5" customWidth="1"/>
-    <col min="12" max="12" width="10" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12" style="5" customWidth="1"/>
-    <col min="14" max="14" width="13" style="5" customWidth="1"/>
-    <col min="15" max="15" width="20" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="7" customWidth="1"/>
+    <col min="7" max="7" width="53.28515625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="42" style="7" customWidth="1"/>
+    <col min="9" max="9" width="24" style="7" customWidth="1"/>
+    <col min="10" max="10" width="32" style="7" customWidth="1"/>
+    <col min="11" max="11" width="22" style="7" customWidth="1"/>
+    <col min="12" max="12" width="10" style="7" customWidth="1"/>
+    <col min="13" max="13" width="12" style="7" customWidth="1"/>
+    <col min="14" max="14" width="13" style="8" customWidth="1"/>
+    <col min="15" max="15" width="30.140625" style="7" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="2"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="2"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="2"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="2"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="2"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="2"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:15" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="2"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="2"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="5"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="5"/>
     </row>
     <row r="10" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="2"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="2"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="2"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="2"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="2"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="5"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="2"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="2"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="5"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="5"/>
     </row>
     <row r="17" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="2"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="5"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="5"/>
     </row>
     <row r="18" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="2"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="5"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="2"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="2"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="2"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="5"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="2"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="2"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="5"/>
     </row>
     <row r="24" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="2"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="5"/>
     </row>
     <row r="25" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="2"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="5"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="2"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="5"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="2"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="5"/>
     </row>
     <row r="28" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M28" s="2"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="2"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="5"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="5"/>
     </row>
     <row r="29" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I29" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="2"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="5"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="5"/>
     </row>
     <row r="30" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="2"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="5"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="5"/>
     </row>
     <row r="31" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="2"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="5"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="2"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="5"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="5"/>
     </row>
     <row r="33" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="2"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="5"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="5"/>
     </row>
     <row r="34" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="2"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="5"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="5"/>
     </row>
     <row r="35" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="2"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M35" s="5"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="5"/>
     </row>
     <row r="36" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="I36" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="2"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" s="5"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="5"/>
     </row>
     <row r="37" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="I37" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="2"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="5"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="5"/>
     </row>
     <row r="38" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I38" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M38" s="2"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="2"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="5"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="5"/>
     </row>
     <row r="39" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="2"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M39" s="5"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="5"/>
     </row>
     <row r="40" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="2"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M40" s="5"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="5"/>
     </row>
     <row r="41" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="2"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="5"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="5"/>
     </row>
     <row r="42" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="A42" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J42" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K42" s="7" t="s">
         <v>259</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M42" s="5" t="s">
+      <c r="M42" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="N42" s="8">
+        <v>46037</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="O42" s="5" t="s">
+      <c r="D43" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="I43" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="J43" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="K43" s="5" t="s">
+      <c r="K43" s="7" t="s">
         <v>259</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M43" s="5" t="s">
+      <c r="M43" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N43" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>263</v>
+      <c r="N43" s="8">
+        <v>46037</v>
+      </c>
+      <c r="O43" s="7" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="J44" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="K44" s="5" t="s">
+      <c r="K44" s="7" t="s">
         <v>259</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="M44" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N44" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="O44" s="5" t="s">
+      <c r="N44" s="8">
+        <v>46037</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="J45" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="K45" s="5" t="s">
+      <c r="K45" s="7" t="s">
         <v>259</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M45" s="5" t="s">
+      <c r="M45" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N45" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="O45" s="5" t="s">
-        <v>263</v>
+      <c r="N45" s="8">
+        <v>46037</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="B46" s="5" t="s">
+      <c r="A46" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="D46" s="5" t="s">
+      <c r="C46" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="G46" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="H46" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="K46" s="5" t="s">
+      <c r="H46" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="K46" s="7" t="s">
         <v>259</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M46" s="5" t="s">
+      <c r="M46" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N46" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="O46" s="5" t="s">
+      <c r="N46" s="8">
+        <v>46037</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="J47" s="7" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="7" t="s">
         <v>259</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M47" s="5" t="s">
+      <c r="M47" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N47" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="O47" s="5" t="s">
-        <v>288</v>
+      <c r="N47" s="8">
+        <v>46037</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="B48" s="5" t="s">
+      <c r="A48" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="C48" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="G48" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="H48" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="H48" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="K48" s="5" t="s">
+      <c r="I48" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="K48" s="7" t="s">
         <v>259</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M48" s="5" t="s">
+      <c r="M48" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N48" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="O48" s="5" t="s">
-        <v>263</v>
+      <c r="N48" s="8">
+        <v>46037</v>
+      </c>
+      <c r="O48" s="7" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="B49" s="5" t="s">
+      <c r="A49" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D49" s="5" t="s">
+      <c r="C49" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D49" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="K49" s="5" t="s">
+      <c r="G49" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="K49" s="7" t="s">
         <v>259</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M49" s="5" t="s">
+      <c r="M49" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N49" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="O49" s="5" t="s">
-        <v>297</v>
+      <c r="N49" s="8">
+        <v>46037</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O49" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A2:O50">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$L2="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:O49">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$L2="Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3423,16 +3474,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3466,7 +3517,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -3480,7 +3531,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B5" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Added and performed test cases around user auth.
</commit_message>
<xml_diff>
--- a/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
+++ b/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB95B003-7625-4826-BBFF-5AF0BD9C1A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163C9051-5781-4D4C-81C3-DADF4EF67F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="359">
   <si>
     <t>TC_ID</t>
   </si>
@@ -968,30 +968,6 @@
   </si>
   <si>
     <t>Blocked</t>
-  </si>
-  <si>
-    <t>TC-041</t>
-  </si>
-  <si>
-    <t>TC-042</t>
-  </si>
-  <si>
-    <t>TC-043</t>
-  </si>
-  <si>
-    <t>TC-044</t>
-  </si>
-  <si>
-    <t>TC-045</t>
-  </si>
-  <si>
-    <t>TC-046</t>
-  </si>
-  <si>
-    <t>TC-047</t>
-  </si>
-  <si>
-    <t>TC-048</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -1018,15 +994,216 @@
   <si>
     <t>Manual API test via Postman. Validates Joi schema on create.</t>
   </si>
+  <si>
+    <t>TC-041-API-01</t>
+  </si>
+  <si>
+    <t>TC-042-API-02</t>
+  </si>
+  <si>
+    <t>TC-043-API-03</t>
+  </si>
+  <si>
+    <t>TC-044-API-04</t>
+  </si>
+  <si>
+    <t>TC-045-API-05</t>
+  </si>
+  <si>
+    <t>TC-046-API-06</t>
+  </si>
+  <si>
+    <t>TC-047-API-07</t>
+  </si>
+  <si>
+    <t>TC-048-API-08</t>
+  </si>
+  <si>
+    <t>TC-049-API-09</t>
+  </si>
+  <si>
+    <t>TC-050-API-10</t>
+  </si>
+  <si>
+    <t>TC-051-API-11</t>
+  </si>
+  <si>
+    <t>TC-052-API-12</t>
+  </si>
+  <si>
+    <t>TC-053-API-13</t>
+  </si>
+  <si>
+    <t>TC-054-API-14</t>
+  </si>
+  <si>
+    <t>TC-055-API-15</t>
+  </si>
+  <si>
+    <t>TC-056-API-16</t>
+  </si>
+  <si>
+    <t>Admin login rejects missing credentials</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>API server running; Postman available</t>
+  </si>
+  <si>
+    <t>1. Send POST /api/auth/login with missing email or password</t>
+  </si>
+  <si>
+    <t>Body:{"email":"", "password":""}</t>
+  </si>
+  <si>
+    <t>Status 400; JSON: success: false and message indicating email/password required.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms early validation before DB/auth logic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual API test via Postman. </t>
+  </si>
+  <si>
+    <t>Admin login fails with invalid credentials (no admin exists)</t>
+  </si>
+  <si>
+    <t>No AdminUser record exists in DB</t>
+  </si>
+  <si>
+    <t>1. Send POST /api/auth/login with any email/password</t>
+  </si>
+  <si>
+    <t>{ "email":"admin@test.com", "password":"Password123!" }</t>
+  </si>
+  <si>
+    <t>401 with { success:false, message:'Invalid credentials.' }</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Generic auth error prevents user enumeration.</t>
+  </si>
+  <si>
+    <t>Create service blocked when not logged in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API </t>
+  </si>
+  <si>
+    <t>Services routes protected with requireAuth and adminOnly; no auth cookie present</t>
+  </si>
+  <si>
+    <t>Send POST /api/services with valid service body</t>
+  </si>
+  <si>
+    <t>{
+  "name": "Bath &amp; Brush",
+  "description": "Bath, blow-dry, brush-out",
+  "image": "https://example.com/service.jpg",
+  "price": 75,
+  "durationMins": 60
+}</t>
+  </si>
+  <si>
+    <t>401 with { success:false, message:'Not authorized.' }</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms auth middleware blocks unauthenticated write access.</t>
+  </si>
+  <si>
+    <t>Update Service blocked when not logged in.</t>
+  </si>
+  <si>
+    <t>Existing service ID available; no auth cookie present</t>
+  </si>
+  <si>
+    <t>PUT /api/services/:id with a valid update payload</t>
+  </si>
+  <si>
+    <t>:id = &lt;existing_service_id&gt;
+Body: { "price": 80 }</t>
+  </si>
+  <si>
+    <t>401 unauthorized response</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms PUT protection.</t>
+  </si>
+  <si>
+    <t>Delete service blocked when ont logged in.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Send </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>DELETE /api/services/:id</t>
+    </r>
+  </si>
+  <si>
+    <t>:id = &lt;existing_service_id&gt;</t>
+  </si>
+  <si>
+    <t>Admin login success sets HttpOnly token cookie</t>
+  </si>
+  <si>
+    <t>AdminUser exists with hashed password; server running</t>
+  </si>
+  <si>
+    <t>POST /api/auth/login with correct credentials Verify response is 200
+Verify response headers include Set-Cookie: token=...; HttpOnly</t>
+  </si>
+  <si>
+    <t>{ "email":"&lt;admin_email&gt;", "password":"&lt;admin_password&gt;" }</t>
+  </si>
+  <si>
+    <t>200 success + token cookie set</t>
+  </si>
+  <si>
+    <t>Create service succeeds when logged in as admin</t>
+  </si>
+  <si>
+    <t>Logged in; token cookie present</t>
+  </si>
+  <si>
+    <t>Login (or reuse cookie session in Postman)
+Send POST /api/services with valid body</t>
+  </si>
+  <si>
+    <t>201 with { success:true, data:&lt;createdService&gt; }</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms full auth + authorization path works.</t>
+  </si>
+  <si>
+    <t>Admin logout clears token cookie</t>
+  </si>
+  <si>
+    <t>Send POST /api/auth/logout
+Verify cookie is cleared
+Try POST /api/services again</t>
+  </si>
+  <si>
+    <t>Logout 200 + subsequent protected route returns 401</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms logout revokes access (client-side).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1053,6 +1230,17 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1101,27 +1289,111 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1439,16 +1711,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q44" sqref="Q44"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="7" customWidth="1"/>
@@ -1466,7 +1738,7 @@
     <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1513,7 +1785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1552,7 +1824,7 @@
       <c r="N2" s="6"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="45" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1591,7 +1863,7 @@
       <c r="N3" s="6"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="45" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -1630,7 +1902,7 @@
       <c r="N4" s="6"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
@@ -1669,7 +1941,7 @@
       <c r="N5" s="6"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="30" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>47</v>
       </c>
@@ -1708,7 +1980,7 @@
       <c r="N6" s="6"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="60" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -1747,7 +2019,7 @@
       <c r="N7" s="6"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="90" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>60</v>
       </c>
@@ -1786,7 +2058,7 @@
       <c r="N8" s="6"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="75" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>66</v>
       </c>
@@ -1825,7 +2097,7 @@
       <c r="N9" s="6"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="135" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -1864,7 +2136,7 @@
       <c r="N10" s="6"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="45" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>80</v>
       </c>
@@ -1903,7 +2175,7 @@
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="60" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>86</v>
       </c>
@@ -1942,7 +2214,7 @@
       <c r="N12" s="6"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="60" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>92</v>
       </c>
@@ -1981,7 +2253,7 @@
       <c r="N13" s="6"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="45" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>98</v>
       </c>
@@ -2020,7 +2292,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="60" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>105</v>
       </c>
@@ -2059,7 +2331,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="60" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>112</v>
       </c>
@@ -2098,7 +2370,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="45" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>118</v>
       </c>
@@ -2137,7 +2409,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="45" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>124</v>
       </c>
@@ -2176,7 +2448,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="60" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>128</v>
       </c>
@@ -2215,7 +2487,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="45" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>133</v>
       </c>
@@ -2254,7 +2526,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="45" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>139</v>
       </c>
@@ -2293,7 +2565,7 @@
       <c r="N21" s="6"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="60" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>146</v>
       </c>
@@ -2332,7 +2604,7 @@
       <c r="N22" s="6"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="60" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>154</v>
       </c>
@@ -2371,7 +2643,7 @@
       <c r="N23" s="6"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="30" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>159</v>
       </c>
@@ -2410,7 +2682,7 @@
       <c r="N24" s="6"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="45" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>164</v>
       </c>
@@ -2449,7 +2721,7 @@
       <c r="N25" s="6"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="60" customHeight="1">
       <c r="A26" s="5" t="s">
         <v>170</v>
       </c>
@@ -2488,7 +2760,7 @@
       <c r="N26" s="6"/>
       <c r="O26" s="5"/>
     </row>
-    <row r="27" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
         <v>176</v>
       </c>
@@ -2527,7 +2799,7 @@
       <c r="N27" s="6"/>
       <c r="O27" s="5"/>
     </row>
-    <row r="28" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="45" customHeight="1">
       <c r="A28" s="5" t="s">
         <v>181</v>
       </c>
@@ -2566,7 +2838,7 @@
       <c r="N28" s="6"/>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="45" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>186</v>
       </c>
@@ -2605,7 +2877,7 @@
       <c r="N29" s="6"/>
       <c r="O29" s="5"/>
     </row>
-    <row r="30" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="45" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>191</v>
       </c>
@@ -2644,7 +2916,7 @@
       <c r="N30" s="6"/>
       <c r="O30" s="5"/>
     </row>
-    <row r="31" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="120" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>197</v>
       </c>
@@ -2683,7 +2955,7 @@
       <c r="N31" s="6"/>
       <c r="O31" s="5"/>
     </row>
-    <row r="32" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="45" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>203</v>
       </c>
@@ -2722,7 +2994,7 @@
       <c r="N32" s="6"/>
       <c r="O32" s="5"/>
     </row>
-    <row r="33" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="45" customHeight="1">
       <c r="A33" s="5" t="s">
         <v>208</v>
       </c>
@@ -2761,7 +3033,7 @@
       <c r="N33" s="6"/>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="45" customHeight="1">
       <c r="A34" s="5" t="s">
         <v>213</v>
       </c>
@@ -2800,7 +3072,7 @@
       <c r="N34" s="6"/>
       <c r="O34" s="5"/>
     </row>
-    <row r="35" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="60" customHeight="1">
       <c r="A35" s="5" t="s">
         <v>217</v>
       </c>
@@ -2839,7 +3111,7 @@
       <c r="N35" s="6"/>
       <c r="O35" s="5"/>
     </row>
-    <row r="36" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="45" customHeight="1">
       <c r="A36" s="5" t="s">
         <v>223</v>
       </c>
@@ -2878,7 +3150,7 @@
       <c r="N36" s="6"/>
       <c r="O36" s="5"/>
     </row>
-    <row r="37" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="45" customHeight="1">
       <c r="A37" s="5" t="s">
         <v>228</v>
       </c>
@@ -2917,7 +3189,7 @@
       <c r="N37" s="6"/>
       <c r="O37" s="5"/>
     </row>
-    <row r="38" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="45" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>233</v>
       </c>
@@ -2956,7 +3228,7 @@
       <c r="N38" s="6"/>
       <c r="O38" s="5"/>
     </row>
-    <row r="39" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="45" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>239</v>
       </c>
@@ -2995,7 +3267,7 @@
       <c r="N39" s="6"/>
       <c r="O39" s="5"/>
     </row>
-    <row r="40" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="45" customHeight="1">
       <c r="A40" s="5" t="s">
         <v>244</v>
       </c>
@@ -3034,7 +3306,7 @@
       <c r="N40" s="6"/>
       <c r="O40" s="5"/>
     </row>
-    <row r="41" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>249</v>
       </c>
@@ -3073,9 +3345,9 @@
       <c r="N41" s="6"/>
       <c r="O41" s="5"/>
     </row>
-    <row r="42" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="30">
       <c r="A42" s="7" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>16</v>
@@ -3117,12 +3389,12 @@
         <v>46037</v>
       </c>
       <c r="O42" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="180">
       <c r="A43" s="7" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>171</v>
@@ -3146,7 +3418,7 @@
         <v>263</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="J43" s="7" t="s">
         <v>264</v>
@@ -3164,12 +3436,12 @@
         <v>46037</v>
       </c>
       <c r="O43" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="75">
       <c r="A44" s="7" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>245</v>
@@ -3211,12 +3483,12 @@
         <v>46037</v>
       </c>
       <c r="O44" s="7" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="30">
       <c r="A45" s="7" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>42</v>
@@ -3258,12 +3530,12 @@
         <v>46037</v>
       </c>
       <c r="O45" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="45">
+      <c r="A46" s="7" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>297</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>245</v>
@@ -3305,12 +3577,12 @@
         <v>46037</v>
       </c>
       <c r="O46" s="7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="45">
       <c r="A47" s="7" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>171</v>
@@ -3352,12 +3624,12 @@
         <v>46037</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="45">
       <c r="A48" s="7" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>171</v>
@@ -3399,12 +3671,12 @@
         <v>46037</v>
       </c>
       <c r="O48" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="45">
       <c r="A49" s="7" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>245</v>
@@ -3446,19 +3718,370 @@
         <v>46037</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>302</v>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="45">
+      <c r="A50" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="K50" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N50" s="8">
+        <v>46040</v>
+      </c>
+      <c r="O50" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="75">
+      <c r="A51" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N51" s="8">
+        <v>46040</v>
+      </c>
+      <c r="O51" s="7" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="165">
+      <c r="A52" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L52" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N52" s="8">
+        <v>46040</v>
+      </c>
+      <c r="O52" s="7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="60">
+      <c r="A53" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N53" s="8">
+        <v>46040</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="30">
+      <c r="A54" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="H54" t="s">
+        <v>343</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N54" s="8">
+        <v>46040</v>
+      </c>
+      <c r="O54" s="7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="75">
+      <c r="A55" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="M55" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="165">
+      <c r="A56" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="O56" s="7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="75">
+      <c r="A57" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="O57" s="7" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:O49" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A2:O50">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="A2:O279">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$L2="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O49">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$L2="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3471,9 +4094,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -3487,7 +4110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -3501,7 +4124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>260</v>
       </c>
@@ -3515,7 +4138,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>291</v>
       </c>
@@ -3529,7 +4152,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>292</v>
       </c>
@@ -3543,7 +4166,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="D6" t="s">
         <v>255</v>
       </c>

</xml_diff>

<commit_message>
Completing testing for routes after logging in with admin credentials.
</commit_message>
<xml_diff>
--- a/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
+++ b/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163C9051-5781-4D4C-81C3-DADF4EF67F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95CF805-1DE9-4CC3-B8E9-538B5CCDD96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="359">
   <si>
     <t>TC_ID</t>
   </si>
@@ -1309,98 +1309,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1713,9 +1622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N58" sqref="N58"/>
+      <selection pane="bottomLeft" activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3990,8 +3899,14 @@
       <c r="K55" s="7" t="s">
         <v>259</v>
       </c>
+      <c r="L55" s="7" t="s">
+        <v>260</v>
+      </c>
       <c r="M55" s="7" t="s">
         <v>261</v>
+      </c>
+      <c r="N55" s="8">
+        <v>46040</v>
       </c>
       <c r="O55" s="7" t="s">
         <v>322</v>
@@ -4031,8 +3946,14 @@
       <c r="K56" s="7" t="s">
         <v>259</v>
       </c>
+      <c r="L56" s="7" t="s">
+        <v>260</v>
+      </c>
       <c r="M56" s="7" t="s">
         <v>261</v>
+      </c>
+      <c r="N56" s="8">
+        <v>46040</v>
       </c>
       <c r="O56" s="7" t="s">
         <v>354</v>
@@ -4069,8 +3990,14 @@
       <c r="K57" s="7" t="s">
         <v>259</v>
       </c>
+      <c r="L57" s="7" t="s">
+        <v>260</v>
+      </c>
       <c r="M57" s="7" t="s">
         <v>261</v>
+      </c>
+      <c r="N57" s="8">
+        <v>46040</v>
       </c>
       <c r="O57" s="7" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
Added three more test cases to test SMS sending.
</commit_message>
<xml_diff>
--- a/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
+++ b/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAD70D2-9057-44F6-8260-DF5189081439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258CE333-FF8A-456E-ADE7-7CBCB44637E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1920" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="393">
   <si>
     <t>TC_ID</t>
   </si>
@@ -1238,6 +1238,69 @@
     <t>GET /api/auth/me returns 200 OK with JSON:
 success: true
 data: { id: &lt;string&gt;, role: "Admin" }</t>
+  </si>
+  <si>
+    <t>TC-058-API-19</t>
+  </si>
+  <si>
+    <t>TC-058-API-20</t>
+  </si>
+  <si>
+    <t>TC-058-API-21</t>
+  </si>
+  <si>
+    <t>Create booking succeeds and triggers SMS (smsStatus=Sent)</t>
+  </si>
+  <si>
+    <t>Server running. Valid service exists. Date/time slot is available (no existing booking for same date+time). Twilio env vars configured. Recipient phone is verified in Twilio (trial).</t>
+  </si>
+  <si>
+    <t>1) In Postman, send POST /api/bookings.\n2) Provide valid payload with verified phone.\n3) Send request.\n4) Verify response + SMS received.</t>
+  </si>
+  <si>
+    <t>serviceId=&lt;VALID_SERVICE_ID&gt;; date=2026-01-20; time=10:00; customerName=Robert Norwood; phone=&lt;VERIFIED_E164_PHONE&gt;; email=test@example.com; notes=Success path</t>
+  </si>
+  <si>
+    <t>Returns 201. Response success=true and booking is created. smsStatus=Sent. smsError empty. SMS confirmation received on phone.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms booking create + Twilio integration works end-to-end.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Validates unique index enforcement on {date, time}.</t>
+  </si>
+  <si>
+    <t>Create booking rejects duplicate date/time slot(409).</t>
+  </si>
+  <si>
+    <t>Server running. Valid service exists. A booking already exists for date=2026-01-20 and time=10:00 (same slot).</t>
+  </si>
+  <si>
+    <t>1) Ensure an existing booking already uses date=2026-01-20 and time=10:00.\n2) In Postman, send POST /api/bookings with the same date/time.\n3) Send request.\n4) Verify conflict response and no new booking created.</t>
+  </si>
+  <si>
+    <t>serviceId=&lt;VALID_SERVICE_ID&gt;; date=2026-01-20; time=10:00; customerName=Jane Doe; phone=&lt;VERIFIED_E164_PHONE&gt;; email=dup@test.com; notes=Duplicate slot test</t>
+  </si>
+  <si>
+    <t>Returns 409 with message "Slot already booked." No new booking created. No SMS sent for the failed request.</t>
+  </si>
+  <si>
+    <t>Server running. Valid service exists. Date/time slot is available. Force SMS failure by using an unverified phone number OR temporarily invalid TWILIO credentials OR remove TWILIO_MESSAGING_SERVICE_SID.</t>
+  </si>
+  <si>
+    <t>Booking succeeds even if SMS fails (smsStatus=Failed, smsError set)</t>
+  </si>
+  <si>
+    <t>1) Intentionally force SMS failure (unverified phone or invalid Twilio env).\n2) In Postman, send POST /api/bookings.\n3) Send request.\n4) Verify booking is still created and smsStatus reflects failure.</t>
+  </si>
+  <si>
+    <t>serviceId=&lt;VALID_SERVICE_ID&gt;; date=2026-01-21; time=11:00; customerName=SMS Fail Test; phone=&lt;UNVERIFIED_OR_INVALID_E164_PHONE&gt;; email=smsfail@test.com; notes=Force SMS failure</t>
+  </si>
+  <si>
+    <t>Returns 201. Booking is created successfully (status remains Confirmed). smsStatus=Failed. smsError contains Twilio error message (or fallback). User does not need SMS success for booking creation.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Validates non-blocking SMS requirement (US-05).</t>
   </si>
 </sst>
 </file>
@@ -1664,11 +1727,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N64" sqref="N64"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4138,6 +4201,129 @@
         <v>366</v>
       </c>
     </row>
+    <row r="60" spans="1:15" ht="135">
+      <c r="A60" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="M60" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N60" s="8">
+        <v>46041</v>
+      </c>
+      <c r="O60" s="7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="135">
+      <c r="A61" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="M61" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N61" s="8">
+        <v>46041</v>
+      </c>
+      <c r="O61" s="7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="135">
+      <c r="A62" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="J62" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="M62" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N62" s="8">
+        <v>46041</v>
+      </c>
+      <c r="O62" s="7" t="s">
+        <v>392</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O49" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>